<commit_message>
integrated story 5 and 8
</commit_message>
<xml_diff>
--- a/MetaMarian_Robot/Data/Config.xlsx
+++ b/MetaMarian_Robot/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.oanea\Documents\IS\MetaMarian\MetaMarian_Robot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EC432E-A363-41F7-89A6-D4D10BD8F7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B67866B-C4C6-411C-9AB6-B65203BFA3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>MTMR_HRCredentials</t>
+  </si>
+  <si>
+    <t>HRCredentials</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -612,7 +618,14 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1614,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>